<commit_message>
More response to reviewers
</commit_message>
<xml_diff>
--- a/rdata/flow_numbers.xlsx
+++ b/rdata/flow_numbers.xlsx
@@ -536,13 +536,13 @@
         <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E2" t="n">
         <v>62</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G2" t="n">
         <v>361</v>

</xml_diff>